<commit_message>
worked on results output and bug fixes
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\MEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0E160-995D-4436-A5A1-45E080224BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E6286-CEB1-45EC-AF50-0B04487E9641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36525" yWindow="2100" windowWidth="28800" windowHeight="15435" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_example" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="78">
   <si>
     <t>MEM case input file</t>
   </si>
@@ -132,9 +132,6 @@
     <t>unmet_demand</t>
   </si>
   <si>
-    <t>non-dispatchable_generator</t>
-  </si>
-  <si>
     <t>generator</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>transmission</t>
   </si>
   <si>
-    <t>node_1_to_2_transmission</t>
-  </si>
-  <si>
     <t>node_2_demand</t>
   </si>
   <si>
@@ -177,12 +171,6 @@
     <t>node_3</t>
   </si>
   <si>
-    <t>node_1_to_3_transmission</t>
-  </si>
-  <si>
-    <t>bidirectional_transmission</t>
-  </si>
-  <si>
     <t>case_name</t>
   </si>
   <si>
@@ -253,6 +241,30 @@
   </si>
   <si>
     <t>Output_Data</t>
+  </si>
+  <si>
+    <t>fixed_generator</t>
+  </si>
+  <si>
+    <t>transfer</t>
+  </si>
+  <si>
+    <t>node_1_to_3_transfer</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>node 1 to 3 one way transfer</t>
+  </si>
+  <si>
+    <t>node 2 to 1 bidirectional transfer</t>
+  </si>
+  <si>
+    <t>node_2_to_1_transmission</t>
+  </si>
+  <si>
+    <t>node_3_curtailment</t>
   </si>
 </sst>
 </file>
@@ -651,15 +663,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735D713C-0288-4607-850D-121F4BB78710}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="49.28515625" customWidth="1"/>
@@ -719,7 +732,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -741,10 +754,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -753,17 +766,17 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -775,7 +788,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -787,7 +800,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -799,7 +812,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -811,7 +824,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -823,7 +836,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
@@ -835,12 +848,12 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="7"/>
@@ -851,8 +864,9 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="10"/>
       <c r="C25" s="7"/>
@@ -863,13 +877,14 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -879,13 +894,14 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -895,13 +911,14 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
@@ -911,10 +928,11 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="7"/>
@@ -925,10 +943,11 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" s="12">
         <v>2005</v>
@@ -941,10 +960,11 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" s="12">
         <v>1</v>
@@ -957,10 +977,11 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B32" s="12">
         <v>1</v>
@@ -973,10 +994,11 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -989,10 +1011,11 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" s="12">
         <v>2005</v>
@@ -1005,13 +1028,14 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35" s="12">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1021,13 +1045,14 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B36" s="12">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1037,10 +1062,11 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B37" s="12">
         <v>24</v>
@@ -1053,10 +1079,11 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B38" s="13">
         <v>9.9999999999999998E+23</v>
@@ -1069,8 +1096,9 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -1081,10 +1109,11 @@
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1095,8 +1124,9 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -1107,8 +1137,9 @@
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>1</v>
       </c>
@@ -1116,10 +1147,10 @@
         <v>29</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>5</v>
@@ -1134,25 +1165,28 @@
         <v>11</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F43" s="2">
         <v>0.03</v>
@@ -1162,7 +1196,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
@@ -1180,7 +1214,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1192,7 +1226,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1200,7 +1234,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -1220,12 +1254,12 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>27</v>
@@ -1242,12 +1276,12 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>27</v>
@@ -1268,10 +1302,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>19</v>
@@ -1291,10 +1325,13 @@
         <v>0.9</v>
       </c>
       <c r="J49" s="2"/>
+      <c r="K49" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>31</v>
@@ -1303,7 +1340,7 @@
         <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -1313,7 +1350,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>32</v>
@@ -1333,17 +1370,17 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -1353,17 +1390,17 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F53" s="2">
         <v>0.03</v>
@@ -1373,94 +1410,101 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>48</v>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2">
-        <v>10</v>
-      </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C56" s="2"/>
+      <c r="C56" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="G56" s="2">
+        <v>10</v>
+      </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
+      <c r="A58" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1471,6 +1515,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
@@ -1589,6 +1634,19 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
working on output + bug fixes
</commit_message>
<xml_diff>
--- a/case_input_example.xlsx
+++ b/case_input_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\MEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E6286-CEB1-45EC-AF50-0B04487E9641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFB1CD6-ECD8-42B0-8911-EDA6ABB3476F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2567C34E-34A1-46AE-A76A-7145792213B5}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>node_1_demand</t>
   </si>
   <si>
-    <t>node_1_unmet_demand</t>
-  </si>
-  <si>
     <t>Note that unmet demand is represented a source with a variable cost only, so unmet demand has an output decision.</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>demand</t>
   </si>
   <si>
-    <t>unmet_demand</t>
-  </si>
-  <si>
     <t>generator</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Name of node from which this technology would get or give its energy (or in the case of transmission, the receiving node)</t>
   </si>
   <si>
-    <t>node_2_unmet_demand</t>
-  </si>
-  <si>
     <t>node_aux</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
     <t>efficiency</t>
   </si>
   <si>
-    <t>One of 'non-dispatchable generator', 'generator', 'curtailment', 'unmet_demand', 'storage',  'transmission', or 'bidirectional_transmission'</t>
-  </si>
-  <si>
     <t>node_3_demand</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>case_name</t>
   </si>
   <si>
-    <t>node_3_unmet_demand</t>
-  </si>
-  <si>
     <t>CASE_DATA</t>
   </si>
   <si>
@@ -265,6 +250,21 @@
   </si>
   <si>
     <t>node_3_curtailment</t>
+  </si>
+  <si>
+    <t>One of 'non-dispatchable generator', 'generator', 'curtailment', 'lost_load', 'storage',  'transmission', or 'bidirectional_transmission'</t>
+  </si>
+  <si>
+    <t>node_1_lost_load</t>
+  </si>
+  <si>
+    <t>lost_load</t>
+  </si>
+  <si>
+    <t>node_2_lost_load</t>
+  </si>
+  <si>
+    <t>node_3_lost_load</t>
   </si>
 </sst>
 </file>
@@ -666,7 +666,7 @@
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,12 +697,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,10 +729,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -754,10 +754,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -766,10 +766,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -853,7 +853,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="7"/>
@@ -881,10 +881,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -898,10 +898,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -915,10 +915,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="11"/>
@@ -932,7 +932,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="7"/>
@@ -947,7 +947,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B30" s="12">
         <v>2005</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B31" s="12">
         <v>1</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B32" s="12">
         <v>1</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B33" s="12">
         <v>1</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B34" s="12">
         <v>2005</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B35" s="12">
         <v>1</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B36" s="12">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B37" s="12">
         <v>24</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B38" s="13">
         <v>9.9999999999999998E+23</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1144,13 +1144,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>5</v>
@@ -1165,28 +1165,28 @@
         <v>11</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>15</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F43" s="2">
         <v>0.03</v>
@@ -1201,7 +1201,7 @@
         <v>20</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>19</v>
@@ -1219,14 +1219,14 @@
         <v>21</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1236,10 +1236,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>19</v>
@@ -1256,13 +1256,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1278,13 +1278,13 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1302,16 +1302,16 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
@@ -1326,21 +1326,21 @@
       </c>
       <c r="J49" s="2"/>
       <c r="K49" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1370,17 +1370,17 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -1390,17 +1390,17 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F53" s="2">
         <v>0.03</v>
@@ -1412,13 +1412,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1430,13 +1430,13 @@
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>19</v>
@@ -1454,18 +1454,18 @@
       </c>
       <c r="J55" s="2"/>
       <c r="K55" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="9"/>

</xml_diff>